<commit_message>
Metabolite class in positive polarity LC-MS.
</commit_message>
<xml_diff>
--- a/Data/NEG_Metabolites_Hetmap.xlsx
+++ b/Data/NEG_Metabolites_Hetmap.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\F4ss0\Documents\Ikiam21062022\Tesis-Pablo-Corella\U_sagittifolia_tubers\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\F4ss0\Documents\Ikiam21062022\Tesis-Pablo-Corella\U_sagittifolia_tubers\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75006333-5A67-4CA8-917B-F52D66726766}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{442B8463-E653-47AE-80A8-DD1D74AC0F65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="345" yWindow="945" windowWidth="20490" windowHeight="10920" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -85491,8 +85491,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D2C99DE-BCF2-4A5C-BDBB-677943C3CC01}">
   <dimension ref="A1:K36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="K32" sqref="K32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>